<commit_message>
Fix typo, update resources
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2205F600-2EAB-432D-9BAF-1D8B7875CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E294612-155B-4331-98F7-3AF115A62FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="930" windowWidth="19425" windowHeight="9675" activeTab="1" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -190,16 +190,10 @@
     <t>&lt;a href="https://www.slideshare.net/kbriney?utm_campaign=profiletracking&amp;utm_medium=sssite&amp;utm_source=ssslideview"&gt;Kristin Briney Slide Share&lt;/a&gt;</t>
   </si>
   <si>
-    <t>University of Pittsburgh Library System</t>
-  </si>
-  <si>
     <t>UK Data Service</t>
   </si>
   <si>
     <t>&lt;a href="https://ukdataservice.ac.uk/learning-hub/"&gt;Learning Hub&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://pitt.libguides.com/managedata/understanding"&gt;Data Management Planning: things to Consider&lt;/a&gt;</t>
   </si>
   <si>
     <t>Stanford Medicine Lane Medical Library</t>
@@ -294,12 +288,6 @@
     <t>&lt;a href="https://docs.google.com/document/d/1u8o5jnWk0Iqp_J06PTu5NjBfVsdoPbBhstht6W0fFp0/edit#heading=h.qjnqq8b54i1d"&gt;Psych-DS: A Technical Specification for Psychological Datasets&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Ldbase</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://www.ldbase.org/resources/best-practices/general-data-management-guidelines"&gt;General Data Management Guidelines&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Reynolds, T., Schatschneider, C. &amp; Logan, J.</t>
   </si>
   <si>
@@ -319,6 +307,9 @@
   </si>
   <si>
     <t>OER Commons - Hubs</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://ukdataservice.ac.uk/learning-hub/research-data-management/plan-to-share/checklist/"&gt;Checklist&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -673,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,40 +722,31 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
-    <sortCondition ref="A2:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B9" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B7" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{C7CD8811-B2D3-4FF7-91ED-FCDDC4F26273}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B8" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -772,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A53E2DC-BA13-40FE-AC98-DC0B21D90DD8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -824,26 +806,26 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +921,7 @@
         <v>2021</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -950,7 +932,7 @@
         <v>2020</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1076,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF00AE3-BFD4-438F-8990-251D0720E643}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,26 +1078,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1105,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1156,7 +1138,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1164,34 +1146,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1232,15 +1214,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1248,18 +1230,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,42 +1254,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add one new resource to blog
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA1C637-8F38-4FE3-B47C-E41209E2625C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95894153-5D74-4042-9E02-6538937E0D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="790" windowWidth="19420" windowHeight="11620" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>&lt;a href="https://www.youtube.com/watch?v=7Ma8WIDinDc&amp;list=PLg5zZXwt2ZW56j8tlEzoSPZPXMRxYLHzu&amp;index=13"&gt;Data Cleaning Principles: Talk for csvconf&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Eaker, C.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://trace.tennessee.edu/cgi/viewcontent.cgi?article=1023&amp;context=utk_libpub"&gt;What Could Possibly Go Wrong? The Impact of Poor Data Management&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -872,10 +878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF588574-DCEC-4E0B-B5D0-93786CE80A13}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,51 +969,63 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B8">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>2021</v>
       </c>
       <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{BFC51063-B290-47C9-BA90-DDEEABDB6F04}"/>
     <hyperlink ref="C6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DC152A6E-AD02-4439-B8DA-F74C8A1774B9}"/>
-    <hyperlink ref="C9" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
+    <hyperlink ref="C10" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
     <hyperlink ref="C2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{B8D202EC-299D-4309-9408-24451F78CCC9}"/>
     <hyperlink ref="C5" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8D4746FE-F3B6-4A3D-ACCA-FFB9D32CE5CF}"/>
-    <hyperlink ref="C8" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
-    <hyperlink ref="C10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
+    <hyperlink ref="C11" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
     <hyperlink ref="C3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{682A5ACB-614C-4F2A-BE8C-8ACBB7384DE1}"/>
     <hyperlink ref="C7" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
+    <hyperlink ref="C8" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1218,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add podcast to blog
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EEDCE5-49DC-4A2C-9FC0-F277040E2BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F9A40A-C439-4EF9-A672-C6A3B7D4BFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>&lt;a href="https://www.povertyactionlab.org/resource/data-cleaning-and-management"&gt;Data cleaning and management&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://anchor.fm/datalibs/episodes/005---A-Targeted-Approach-to-Outreach-and-Instruction-at-UC-Berkeley---Sackmann--Smith---Neeser-e1mek11?%24web_only=true&amp;_branch_match_id=1128746294660517070&amp;utm_source=web&amp;utm_campaign=web-share&amp;utm_medium=sharing&amp;_branch_referrer=H4sIAAAAAAAAA8soKSkottLXLy7IL8lMq0zMS87IL9ItT03SSywo0MvJzMvWT9V3MTXJ90%2B1zDEpSQIA16lMVTAAAAA%3D"&gt;IDEA: Improving Data Engagement and Advocacy&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -706,9 +709,9 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -716,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -724,7 +727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -732,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -740,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -748,7 +751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -756,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -764,7 +767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -794,13 +797,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.453125" customWidth="1"/>
+    <col min="2" max="2" width="64.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -808,7 +811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -816,7 +819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -824,7 +827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -832,7 +835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -840,7 +843,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -848,7 +851,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -856,7 +859,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -864,7 +867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -899,13 +902,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="170.7109375" customWidth="1"/>
+    <col min="1" max="2" width="33.54296875" customWidth="1"/>
+    <col min="3" max="3" width="170.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -916,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -927,7 +930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -938,7 +941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -949,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -960,7 +963,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -971,7 +974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -982,7 +985,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -993,7 +996,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1054,13 +1057,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1110,13 +1113,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1181,19 +1184,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83599360-7CC5-4FEC-96E9-4F9BDB149781}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1233,33 +1236,42 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B6">
-    <sortCondition ref="A2:A6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+    <sortCondition ref="A2:A7"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{90272032-5A67-4990-B442-C6BD8299E43E}"/>
     <hyperlink ref="B2" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{D8EC5363-580E-427B-B7D1-0E9DDFAEC174}"/>
-    <hyperlink ref="B6" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
     <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{7E3B9977-AC69-49A1-ABF4-47BB4499BAB1}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
     <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{967C7D96-CFB3-4000-AFED-F0210BC4FE4E}"/>
+    <hyperlink ref="B6" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{C62F1CA3-935E-41C9-9AB7-B20FAA337BEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1269,17 +1281,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1311,7 +1323,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1327,7 +1339,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1351,7 +1363,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -1375,7 +1387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Update resources blog post
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C68F9C0-42CF-43FE-931B-90B33CCAB152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DED161-64F3-4590-84C5-2B94692AD287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -73,9 +73,6 @@
     <t>&lt;a href="https://www.icpsr.umich.edu/files/deposit/dataprep.pdf"&gt;Guide to Social Science Data Preparation and Archiving&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://cghlewis.github.io/mpsi-data-training/index.html"&gt;Data Management in Large-Scale Education Research&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
   </si>
   <si>
     <t>&lt;a href="https://povertyaction.github.io/guides/cleaning/readme/"&gt;Cleaning Guide&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://cghlewis.github.io/mpsi-data-training/training_4.html"&gt;Data Cleaning Plan&lt;/a&gt;</t>
   </si>
   <si>
     <t>Broman, K. &amp; Woo, K.</t>
@@ -276,9 +270,6 @@
     <t>Borer, E., Seabloom, E., Jones, M. &amp; Schildhauer, M.*</t>
   </si>
   <si>
-    <t>Crystal Lewis*</t>
-  </si>
-  <si>
     <t>Kline, et al.</t>
   </si>
   <si>
@@ -411,10 +402,16 @@
     <t xml:space="preserve">Crystal Lewis </t>
   </si>
   <si>
-    <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://drive.google.com/drive/folders/1lRKEx_uMhbzcLeVZZBPX6_amde5uYuvf"&gt;Checklists&lt;/a&gt;</t>
+    <t>&lt;a href="https://datamgmtinedresearch.com/&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://osf.io/e5g6t/"&gt;Checklists&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing Blog Post&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://cghlewis.github.io/ncme-data-cleaning-workshop/"&gt;Data Cleaning for Data Sharing Workshop Materials&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -772,7 +769,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,10 +784,10 @@
     </row>
     <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -798,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -811,15 +808,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -835,18 +832,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -877,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A53E2DC-BA13-40FE-AC98-DC0B21D90DD8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -889,74 +886,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -997,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1005,123 +1002,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>2021</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>2009</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>2021</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>2020</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>2016</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>2022</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>2021</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1169,42 +1166,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1223,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF00AE3-BFD4-438F-8990-251D0720E643}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1246,39 +1243,39 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1309,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1320,58 +1317,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1396,7 +1393,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1415,122 +1412,122 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
         <v>121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
         <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1563,7 +1560,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1582,42 +1579,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update links in blog post
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DED161-64F3-4590-84C5-2B94692AD287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1163EB05-437A-47D5-91F6-7F17265F4E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t xml:space="preserve">Crystal Lewis </t>
   </si>
   <si>
-    <t>&lt;a href="https://datamgmtinedresearch.com/&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href="https://osf.io/e5g6t/"&gt;Checklists&lt;/a&gt;</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>&lt;a href="https://cghlewis.github.io/ncme-data-cleaning-workshop/"&gt;Data Cleaning for Data Sharing Workshop Materials&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://datamgmtinedresearch.com/"&gt;Data Management in Large-Scale Education Research Book&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -874,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A53E2DC-BA13-40FE-AC98-DC0B21D90DD8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1243,7 +1243,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1439,7 +1439,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1447,7 +1447,7 @@
         <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Remove bad link from blog post
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1163EB05-437A-47D5-91F6-7F17265F4E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46AEA0B-50C1-4779-ACDA-ED2FBC8D66C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>&lt;a href="https://rdmkit.elixir-europe.org/"&gt;Research Data Management Kit&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://the-turing-way.netlify.app/welcome"&gt;Guide&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;a href="https://ies.ed.gov/ncee/pubs/2022004/pdf/2022004.pdf"&gt;Sharing Study Data: A Guide for Education Researchers&lt;/a&gt;</t>
@@ -339,12 +336,6 @@
     <t>Borghi, J., Abrams, S., Lowenberg, D., Simms, S. &amp; Chodacki, J.</t>
   </si>
   <si>
-    <t>Johns Hopkins Institute for Clinical and Translational Research (ICTR)</t>
-  </si>
-  <si>
-    <t>&lt;a href="https://ictrweb.johnshopkins.edu/ictr/dmig/Best_Practice/home.html?v=65849"&gt;Best Practices for Research Data Management&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>J-PAL</t>
   </si>
   <si>
@@ -412,6 +403,9 @@
   </si>
   <si>
     <t>&lt;a href="https://datamgmtinedresearch.com/"&gt;Data Management in Large-Scale Education Research Book&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://the-turing-way.netlify.app/welcome"&gt;Handbook&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -766,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,10 +778,10 @@
     </row>
     <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -795,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -808,18 +802,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -827,46 +821,37 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
+    <sortCondition ref="A2:A9"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B10" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B9" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{17E17D06-812D-4223-9000-D327BBFA127E}"/>
-    <hyperlink ref="B5" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B9" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B8" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -886,74 +871,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -994,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1002,123 +987,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>2021</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>2009</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>2021</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>2020</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>2016</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>2022</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>2021</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1166,42 +1151,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1243,39 +1228,39 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1309,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1317,58 +1302,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
         <v>88</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1412,26 +1397,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
         <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1439,95 +1424,95 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
         <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
         <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1579,42 +1564,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix citations in resources
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46AEA0B-50C1-4779-ACDA-ED2FBC8D66C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5398FC92-B705-43EC-BFFD-8C35B8427186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="2" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Institute of Education Sciences</t>
   </si>
   <si>
-    <t>Crystal Lewis</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>&lt;a href="https://figshare.com/articles/presentation/Data_Sharing_and_Data_Shared/15040740"&gt;Data Sharing and Data Shared&lt;/a&gt;</t>
   </si>
   <si>
-    <t>All slides available from Kristin Briney</t>
-  </si>
-  <si>
     <t>&lt;a href="https://www.slideshare.net/kbriney?utm_campaign=profiletracking&amp;utm_medium=sssite&amp;utm_source=ssslideview"&gt;Kristin Briney Slide Share&lt;/a&gt;</t>
   </si>
   <si>
@@ -199,9 +193,6 @@
     <t>&lt;a href="https://datamanagement.hms.harvard.edu/about/what-research-data-management/biomedical-data-lifecycle"&gt;Research Data Management Checklist&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Kristin Briney</t>
-  </si>
-  <si>
     <t>&lt;a href="https://figshare.com/articles/poster/Data_Management_Plan_Checklist/1130852"&gt;Data Management Plan Checklist&lt;/a&gt;</t>
   </si>
   <si>
@@ -245,9 +236,6 @@
   </si>
   <si>
     <t>&lt;a href="https://www.acaps.org/sites/acaps/files/resources/files/acaps_technical_brief_data_cleaning_april_2016_0.pdf"&gt;Data Cleaning&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Karl Broman</t>
   </si>
   <si>
     <t>&lt;a href="https://kbroman.org/steps2rr/"&gt;Steps toward reproducible research&lt;/a&gt;</t>
@@ -267,9 +255,6 @@
     <t>Borer, E., Seabloom, E., Jones, M. &amp; Schildhauer, M.*</t>
   </si>
   <si>
-    <t>Kline, et al.</t>
-  </si>
-  <si>
     <t>&lt;a href="https://docs.google.com/document/d/1u8o5jnWk0Iqp_J06PTu5NjBfVsdoPbBhstht6W0fFp0/edit#heading=h.qjnqq8b54i1d"&gt;Psych-DS: A Technical Specification for Psychological Datasets&lt;/a&gt;</t>
   </si>
   <si>
@@ -390,12 +375,6 @@
     <t>&lt;a href="https://cghlewis.com/talk/uhcl/"&gt;Data Management Workflows for Education Research Studies&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Crystal Lewis </t>
-  </si>
-  <si>
-    <t>&lt;a href="https://osf.io/e5g6t/"&gt;Checklists&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href="https://cghlewis.com/blog/data_clean_01/"&gt;Data Cleaning for Data Sharing Blog Post&lt;/a&gt;</t>
   </si>
   <si>
@@ -406,6 +385,36 @@
   </si>
   <si>
     <t>&lt;a href="https://the-turing-way.netlify.app/welcome"&gt;Handbook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://osf.io/e5g6t/"&gt;Checklists for every phase of a project&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://prezi.com/p/mku89urakpnn/systematic-data-validation/"&gt;Data Validation&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Briney, K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broman, K.  </t>
+  </si>
+  <si>
+    <t>DeCoster, J.</t>
+  </si>
+  <si>
+    <t>Data Structure Standard</t>
+  </si>
+  <si>
+    <t>Schatschneider, C., Edwards, A., &amp; Shero, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://figshare.com/articles/preprint/De-Identification_Guide/13228664/2"&gt;De-identification Guide&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Wilson, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1005510"&gt;Good Enough Practices in Scientific Computing&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -762,74 +771,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -837,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -845,10 +854,10 @@
     <sortCondition ref="A2:A9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
     <hyperlink ref="B9" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
     <hyperlink ref="B8" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -871,74 +880,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -962,10 +971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF588574-DCEC-4E0B-B5D0-93786CE80A13}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,134 +985,145 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>2021</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>2009</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>2021</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>2020</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>2016</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>2022</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>2021</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13">
+        <v>2017</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1122,6 +1142,7 @@
     <hyperlink ref="C8" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
     <hyperlink ref="C9" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
     <hyperlink ref="C5" r:id="rId11" display="https://rdmkit.elixir-europe.org/" xr:uid="{529A61DE-AC1F-4EC6-90AD-966DB5394FEE}"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1132,7 +1153,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,59 +1164,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
-    <hyperlink ref="B6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
-    <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{DB660BFF-32D8-4552-ADE1-A22912433FF8}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{57D36F4D-5ECB-424B-8CAE-D6BD44420EF1}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
+    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1206,7 +1227,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1217,50 +1238,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1271,8 +1292,8 @@
     <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{FA35CA7A-1BB9-4222-B36D-6AA4AF1AFB40}"/>
     <hyperlink ref="B5" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{4AAD8AF4-DD2A-4FBD-BD12-663C4FCEE09D}"/>
     <hyperlink ref="B3" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{09326CED-43A5-4B07-8756-EC90B5BA4D4A}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{AEB48163-745F-49B3-AAFA-B775BED64A89}"/>
-    <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{7CFA00F0-7017-4EE8-ACA3-9DA1BA5BF9EB}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{AEB48163-745F-49B3-AAFA-B775BED64A89}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{7CFA00F0-7017-4EE8-ACA3-9DA1BA5BF9EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1280,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83599360-7CC5-4FEC-96E9-4F9BDB149781}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1294,80 +1315,89 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-    <sortCondition ref="A2:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{90272032-5A67-4990-B442-C6BD8299E43E}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{90272032-5A67-4990-B442-C6BD8299E43E}"/>
     <hyperlink ref="B2" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{D8EC5363-580E-427B-B7D1-0E9DDFAEC174}"/>
-    <hyperlink ref="B7" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
+    <hyperlink ref="B8" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{BCF07CDC-44C2-4BC3-A669-49A65B574C1A}"/>
     <hyperlink ref="B3" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{7E3B9977-AC69-49A1-ABF4-47BB4499BAB1}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
-    <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{967C7D96-CFB3-4000-AFED-F0210BC4FE4E}"/>
-    <hyperlink ref="B6" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{C62F1CA3-935E-41C9-9AB7-B20FAA337BEC}"/>
+    <hyperlink ref="B9" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{E1A2CF24-262B-426D-BD8E-FD5C95E7EDDC}"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{967C7D96-CFB3-4000-AFED-F0210BC4FE4E}"/>
+    <hyperlink ref="B7" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{C62F1CA3-935E-41C9-9AB7-B20FAA337BEC}"/>
+    <hyperlink ref="B4" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1375,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,31 +1419,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
@@ -1421,120 +1451,129 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
-    <hyperlink ref="B11" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{BF5DB17B-A2E9-4364-9EA8-EAFDC95D0D19}"/>
+    <hyperlink ref="B14" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B7E8A39-208D-4BAB-BD0E-C476EEF71874}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{17FB9F7C-2EEB-420C-AD50-8F5369FBC4E8}"/>
     <hyperlink ref="B2" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8736C4FB-ED40-4AAA-A513-1B3997C412A1}"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
+    <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
     <hyperlink ref="B3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{6400C49C-6A30-43A4-8FD2-3A23E629EA75}"/>
-    <hyperlink ref="B15" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{7497676C-A29B-4896-B50B-F18E6702CD8C}"/>
-    <hyperlink ref="B16" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
-    <hyperlink ref="B8" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
-    <hyperlink ref="B12" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
-    <hyperlink ref="B7" r:id="rId14" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
-    <hyperlink ref="B6" r:id="rId15" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+    <hyperlink ref="B16" r:id="rId9" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
+    <hyperlink ref="B9" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
+    <hyperlink ref="B5" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B8" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+    <hyperlink ref="B7" r:id="rId15" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1545,7 +1584,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1556,50 +1595,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a few additional resources
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2270101C-218A-48CC-9A64-FD3E0B464360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15BC19-A9A2-45E6-A79A-D1240CBCDA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="132">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -252,9 +252,6 @@
 Library Consultancy&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Borer, E., Seabloom, E., Jones, M. &amp; Schildhauer, M.*</t>
-  </si>
-  <si>
     <t>&lt;a href="https://docs.google.com/document/d/1u8o5jnWk0Iqp_J06PTu5NjBfVsdoPbBhstht6W0fFp0/edit#heading=h.qjnqq8b54i1d"&gt;Psych-DS: A Technical Specification for Psychological Datasets&lt;/a&gt;</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>&lt;a href="https://figshare.com/articles/preprint/The_Basics_of_Data_Management/13215350"&gt;The Basics of Data Management&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Reynolds, T., Schatschneider, C. &amp; Logan, J.*</t>
-  </si>
-  <si>
     <t>Search "data management" in repository databases for great resources</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
     <t>&lt;a href="https://doi.org/10.3897/rio.4.e26439"&gt;Support Your Data: A Research Data Management Guide for Researchers&lt;/a&gt;</t>
   </si>
   <si>
-    <t>J-Pal*</t>
-  </si>
-  <si>
     <t>Urban Institute</t>
   </si>
   <si>
@@ -415,6 +406,39 @@
   </si>
   <si>
     <t>&lt;a href="https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1005510"&gt;Good Enough Practices in Scientific Computing&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://dimewiki.worldbank.org/Primary_Data_Collection"&gt;Dimewiki&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>DIME Analytics</t>
+  </si>
+  <si>
+    <t>Filip, A.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.sjsu.edu/research/docs/irb-data-management-handbook.pdf"&gt;Data Management Handbook for Human Subjects Research&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Yenni, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://journals.plos.org/plosbiology/article?id=10.1371/journal.pbio.3000125"&gt;Developing a modern data workflow for regularly updated data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>J-Pal</t>
+  </si>
+  <si>
+    <t>White, et al.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://ojs.library.queensu.ca/index.php/IEE/article/view/4608"&gt;Nine simple ways to make it easier to (re)use your data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Towse, A., Ellis, D., Towse, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.tandfonline.com/doi/full/10.1080/00224545.2021.1938811"&gt;Making data meaningful: guidelines for good quality open data&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -769,15 +793,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -785,7 +809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -793,74 +817,92 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
-        <v>113</v>
+      <c r="B11" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
-    <sortCondition ref="A2:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B9" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B8" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
+    <hyperlink ref="B11" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B10" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -872,13 +914,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.453125" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -886,7 +928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -894,7 +936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -902,7 +944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -910,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -918,23 +960,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -942,7 +984,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -974,16 +1016,16 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.54296875" customWidth="1"/>
-    <col min="3" max="3" width="170.7265625" customWidth="1"/>
+    <col min="1" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="170.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -994,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1005,132 +1047,132 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>2009</v>
+        <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="B4">
+        <v>2018</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8">
+        <v>2016</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
         <v>2022</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5">
-        <v>2018</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
         <v>2021</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8">
-        <v>2020</v>
-      </c>
-      <c r="C8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9">
-        <v>2016</v>
-      </c>
-      <c r="C9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>2022</v>
-      </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B12">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{BFC51063-B290-47C9-BA90-DDEEABDB6F04}"/>
-    <hyperlink ref="C7" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DC152A6E-AD02-4439-B8DA-F74C8A1774B9}"/>
-    <hyperlink ref="C11" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{BFC51063-B290-47C9-BA90-DDEEABDB6F04}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://rdmkit.elixir-europe.org/" xr:uid="{DC152A6E-AD02-4439-B8DA-F74C8A1774B9}"/>
+    <hyperlink ref="C10" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{C2CCC9A4-192D-4723-A6B9-1DD8433A4B7B}"/>
     <hyperlink ref="C2" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{B8D202EC-299D-4309-9408-24451F78CCC9}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8D4746FE-F3B6-4A3D-ACCA-FFB9D32CE5CF}"/>
-    <hyperlink ref="C10" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
-    <hyperlink ref="C12" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
-    <hyperlink ref="C3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{682A5ACB-614C-4F2A-BE8C-8ACBB7384DE1}"/>
-    <hyperlink ref="C8" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
-    <hyperlink ref="C9" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
-    <hyperlink ref="C5" r:id="rId11" display="https://rdmkit.elixir-europe.org/" xr:uid="{529A61DE-AC1F-4EC6-90AD-966DB5394FEE}"/>
+    <hyperlink ref="C5" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{8D4746FE-F3B6-4A3D-ACCA-FFB9D32CE5CF}"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{FFCD0CA1-5CD9-45D3-A226-A36829343339}"/>
+    <hyperlink ref="C11" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{1E20410E-725C-4F71-8819-F507842316CA}"/>
+    <hyperlink ref="C7" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{64132426-ED00-4A25-8720-0CBAF1564A6A}"/>
+    <hyperlink ref="C8" r:id="rId9" display="https://rdmkit.elixir-europe.org/" xr:uid="{206910D2-EE19-4E82-989E-46F2C4254F4A}"/>
+    <hyperlink ref="C4" r:id="rId10" display="https://rdmkit.elixir-europe.org/" xr:uid="{529A61DE-AC1F-4EC6-90AD-966DB5394FEE}"/>
+    <hyperlink ref="C12" r:id="rId11" display="https://rdmkit.elixir-europe.org/" xr:uid="{A17A33C1-790D-41EB-9DA4-9C2579AE1D3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1144,13 +1186,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1158,31 +1200,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1190,7 +1232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1218,13 +1260,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1232,15 +1274,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1248,15 +1290,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1264,12 +1306,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1292,16 +1334,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1309,7 +1351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1317,7 +1359,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1325,23 +1367,23 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1349,15 +1391,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1365,12 +1407,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1393,19 +1435,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1421,31 +1463,31 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1453,31 +1495,31 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1485,7 +1527,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1493,7 +1535,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1501,57 +1543,65 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
         <v>107</v>
       </c>
-      <c r="B14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
         <v>120</v>
       </c>
-      <c r="B17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>123</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
@@ -1562,15 +1612,16 @@
     <hyperlink ref="B4" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{1B0A27D1-7156-47C3-ABDA-1CF3B2E67444}"/>
     <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{B13D64B1-BDC7-4011-9B1D-F84D68D1B179}"/>
     <hyperlink ref="B3" r:id="rId8" display="https://rdmkit.elixir-europe.org/" xr:uid="{6400C49C-6A30-43A4-8FD2-3A23E629EA75}"/>
-    <hyperlink ref="B16" r:id="rId9" display="https://the-turing-way.netlify.app/welcome" xr:uid="{58B0795A-28FC-46B1-AAC3-E406B300BDA2}"/>
-    <hyperlink ref="B9" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
-    <hyperlink ref="B5" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
-    <hyperlink ref="B8" r:id="rId13" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
-    <hyperlink ref="B7" r:id="rId15" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
+    <hyperlink ref="B9" r:id="rId9" display="https://the-turing-way.netlify.app/welcome" xr:uid="{848F7200-0B87-4F29-A4AF-65BF4B17FB1E}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://the-turing-way.netlify.app/welcome" xr:uid="{0920355D-AE8B-41F9-B48D-C874B53FAF91}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://the-turing-way.netlify.app/welcome" xr:uid="{5842F03B-43C3-49FE-A94E-760606629084}"/>
+    <hyperlink ref="B8" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
+    <hyperlink ref="B7" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
+    <hyperlink ref="B19" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
+    <hyperlink ref="B17" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1581,16 +1632,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="42.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1598,44 +1649,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update two more links in resource blog
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15BC19-A9A2-45E6-A79A-D1240CBCDA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C37265-3E7C-42F4-81B5-C60399859AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -408,9 +408,6 @@
     <t>&lt;a href="https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1005510"&gt;Good Enough Practices in Scientific Computing&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href="https://dimewiki.worldbank.org/Primary_Data_Collection"&gt;Dimewiki&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>DIME Analytics</t>
   </si>
   <si>
@@ -439,6 +436,15 @@
   </si>
   <si>
     <t>&lt;a href="https://www.tandfonline.com/doi/full/10.1080/00224545.2021.1938811"&gt;Making data meaningful: guidelines for good quality open data&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Responsible Data</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://responsibledata.io/resources/handbook/"&gt;The Handbook of the Modern Development Specialist&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://dimewiki.worldbank.org/Main_Page"&gt;DIME Wiki&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -793,15 +799,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -809,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -817,15 +823,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -833,15 +839,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
         <v>123</v>
       </c>
-      <c r="B5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -849,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -857,7 +863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -865,7 +871,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -873,36 +879,45 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B11" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B10" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B11" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
     <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
     <hyperlink ref="B3" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
     <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -914,13 +929,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.453125" customWidth="1"/>
+    <col min="2" max="2" width="64.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -928,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -936,7 +951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -944,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -952,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -960,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -968,7 +983,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -976,7 +991,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -984,7 +999,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1019,13 +1034,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="170.7109375" customWidth="1"/>
+    <col min="1" max="2" width="33.54296875" customWidth="1"/>
+    <col min="3" max="3" width="170.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1080,7 +1095,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1102,7 +1117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1113,7 +1128,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1124,7 +1139,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1135,7 +1150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1146,15 +1161,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12">
         <v>2019</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1186,13 +1201,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1200,7 +1215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1232,7 +1247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1260,13 +1275,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1282,7 +1297,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1298,7 +1313,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1306,7 +1321,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1337,13 +1352,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1351,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1359,7 +1374,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1375,7 +1390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1383,7 +1398,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1391,7 +1406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1407,7 +1422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1437,17 +1452,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1495,7 +1510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1503,7 +1518,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1511,7 +1526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1519,7 +1534,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1527,7 +1542,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1535,7 +1550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1543,15 +1558,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1559,7 +1574,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -1575,23 +1590,23 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
         <v>128</v>
       </c>
-      <c r="B18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -1635,13 +1650,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1649,7 +1664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1657,7 +1672,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1673,7 +1688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1681,7 +1696,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Add POWER slides to blog resources
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C37265-3E7C-42F4-81B5-C60399859AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5943AD0-C51D-4071-BC05-143EE1AE805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="136">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>&lt;a href="https://dimewiki.worldbank.org/Main_Page"&gt;DIME Wiki&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>POWER Data Management Hub</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://osf.io/ap3tk/"&gt;Slides from hub presenters&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -801,13 +807,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -815,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -823,7 +829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -831,7 +837,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -839,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -847,7 +853,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -855,7 +861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -863,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -871,7 +877,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -879,7 +885,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -887,7 +893,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -895,7 +901,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -929,13 +935,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.453125" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -943,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -951,7 +957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -959,7 +965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -967,7 +973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -975,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -983,7 +989,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -991,7 +997,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1034,13 +1040,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.54296875" customWidth="1"/>
-    <col min="3" max="3" width="170.7265625" customWidth="1"/>
+    <col min="1" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="170.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -1195,19 +1201,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314F75B-5804-4835-9447-15ECE75CB0EC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1247,12 +1253,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1262,6 +1276,7 @@
     <hyperlink ref="B5" r:id="rId3" display="https://rdmkit.elixir-europe.org/" xr:uid="{F9369E95-DB00-415B-9C4E-26398D2D43ED}"/>
     <hyperlink ref="B4" r:id="rId4" display="https://rdmkit.elixir-europe.org/" xr:uid="{31BEDC47-DAD5-48A5-9285-FE7C7BAF828A}"/>
     <hyperlink ref="B3" r:id="rId5" display="https://rdmkit.elixir-europe.org/" xr:uid="{F2BB4DDC-F382-4471-AE08-8FFB6600BC49}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{D7E37755-9937-447D-B08A-D8A38C20E831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1275,13 +1290,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1289,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1305,7 +1320,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1313,7 +1328,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1321,7 +1336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1352,13 +1367,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1374,7 +1389,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1382,7 +1397,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1398,7 +1413,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1406,7 +1421,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1414,7 +1429,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1422,7 +1437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1456,13 +1471,13 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1478,7 +1493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1486,7 +1501,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -1494,7 +1509,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1510,7 +1525,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1518,7 +1533,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1526,7 +1541,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1542,7 +1557,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1550,7 +1565,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1558,7 +1573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1574,7 +1589,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1582,7 +1597,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -1590,7 +1605,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -1598,7 +1613,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -1606,7 +1621,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -1650,13 +1665,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="42.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1672,7 +1687,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1680,7 +1695,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1688,7 +1703,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1696,7 +1711,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Add resource to blog post
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5943AD0-C51D-4071-BC05-143EE1AE805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2129D4-0E10-4505-A25D-4F41288F9B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -451,14 +451,25 @@
   </si>
   <si>
     <t>&lt;a href="https://osf.io/ap3tk/"&gt;Slides from hub presenters&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://caltechlibrary.github.io/RDMworkbook/"&gt;The Research Data Management Workbook&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -486,11 +497,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,15 +817,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="52.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -821,106 +833,115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>122</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>90</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
-    <hyperlink ref="B12" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
-    <hyperlink ref="B11" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
-    <hyperlink ref="B3" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
-    <hyperlink ref="B5" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{10FFB09D-AF0A-46D6-8B41-EF7CF92A5F82}"/>
+    <hyperlink ref="B13" r:id="rId2" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E3CBD86C-F63A-419C-AE39-BD7935BC27E8}"/>
+    <hyperlink ref="B12" r:id="rId3" display="https://the-turing-way.netlify.app/welcome" xr:uid="{E95189EF-1904-402F-A49D-48950187DABD}"/>
+    <hyperlink ref="B9" r:id="rId4" display="https://the-turing-way.netlify.app/welcome" xr:uid="{3DA8228C-B70B-4E56-A9A2-41A1E036809E}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://the-turing-way.netlify.app/welcome" xr:uid="{D22F0176-8B44-4C40-AF7C-4A1A2E32B8B4}"/>
+    <hyperlink ref="B6" r:id="rId6" display="https://rdmkit.elixir-europe.org/" xr:uid="{EF7E737D-19B2-4BBC-83BA-8A78418603AB}"/>
+    <hyperlink ref="B11" r:id="rId7" display="https://rdmkit.elixir-europe.org/" xr:uid="{3B35D87F-70F7-4DF3-BECE-762D44177028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -935,13 +956,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.453125" customWidth="1"/>
+    <col min="2" max="2" width="64.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -949,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -957,7 +978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -965,7 +986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -973,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -981,7 +1002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -989,7 +1010,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -997,7 +1018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1005,7 +1026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1040,13 +1061,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="170.7109375" customWidth="1"/>
+    <col min="1" max="2" width="33.54296875" customWidth="1"/>
+    <col min="3" max="3" width="170.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1100,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1090,7 +1111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1101,7 +1122,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1112,7 +1133,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1123,7 +1144,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1134,7 +1155,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1145,7 +1166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1156,7 +1177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1167,7 +1188,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -1203,17 +1224,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314F75B-5804-4835-9447-15ECE75CB0EC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1229,7 +1250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1237,7 +1258,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1245,7 +1266,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1253,7 +1274,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -1290,13 +1311,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1320,7 +1341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1328,7 +1349,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1336,7 +1357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1367,13 +1388,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1381,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1389,7 +1410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1397,7 +1418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1405,7 +1426,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1413,7 +1434,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1421,7 +1442,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1429,7 +1450,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1437,7 +1458,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1471,13 +1492,13 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1493,7 +1514,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +1522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1517,7 +1538,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1525,7 +1546,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1541,7 +1562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1557,7 +1578,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1565,7 +1586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1573,7 +1594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1589,7 +1610,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1597,7 +1618,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -1605,7 +1626,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -1613,7 +1634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -1621,7 +1642,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -1665,13 +1686,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1687,7 +1708,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1695,7 +1716,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1703,7 +1724,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1711,7 +1732,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Add data mgmt resource
</commit_message>
<xml_diff>
--- a/content/blog/data_mgmt_resources/resources.xlsx
+++ b/content/blog/data_mgmt_resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\data_mgmt_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2129D4-0E10-4505-A25D-4F41288F9B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B57EE7C-2134-45AE-96B1-50CFAD216C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="6" xr2:uid="{6BAE7F57-3725-4351-837E-8E947D95CD51}"/>
   </bookViews>
   <sheets>
     <sheet name="guides" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <t>The Turing Way</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>&lt;a href="https://caltechlibrary.github.io/RDMworkbook/"&gt;The Research Data Management Workbook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Morrow, J.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.slideshare.net/slideshow/brief-introduction-to-the-12-steps-of-evaluagio/26168236#4"&gt;Brief Introduction to the 12 Steps of Evaluation Data Cleaning&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -819,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4B91C1-22BD-4BE1-B1F3-299A92712ADB}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1486,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3A241-81BA-45F4-A464-40BCF2B4B4F0}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,39 +1626,47 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>119</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://rdmkit.elixir-europe.org/" xr:uid="{7A5B84E9-93F3-4801-AFDD-33E1F49AA98D}"/>
@@ -1669,10 +1683,11 @@
     <hyperlink ref="B8" r:id="rId12" display="https://the-turing-way.netlify.app/welcome" xr:uid="{B98841DC-A144-4DA0-8636-26565DF68AFD}"/>
     <hyperlink ref="B15" r:id="rId13" display="https://rdmkit.elixir-europe.org/" xr:uid="{6B9E2779-1F65-4F62-9A7F-E809F81333D3}"/>
     <hyperlink ref="B7" r:id="rId14" display="https://rdmkit.elixir-europe.org/" xr:uid="{9F3CBAC0-B921-4DE2-A65A-B7E86FD49EDC}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
-    <hyperlink ref="B17" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://the-turing-way.netlify.app/welcome" xr:uid="{A35D5C69-8E3B-4FAA-9C5E-233488621C17}"/>
+    <hyperlink ref="B20" r:id="rId16" display="https://rdmkit.elixir-europe.org/" xr:uid="{F7DC8ACB-8501-4D8A-8D18-362905B75F1D}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://the-turing-way.netlify.app/welcome" xr:uid="{8D02884E-C75F-488F-B501-3D966342F33D}"/>
+    <hyperlink ref="B18" r:id="rId18" display="https://rdmkit.elixir-europe.org/" xr:uid="{C98846A5-CA26-45F3-ACCE-26115E7B9672}"/>
+    <hyperlink ref="B16" r:id="rId19" display="https://rdmkit.elixir-europe.org/" xr:uid="{D1FE705A-5C82-4CEA-B5B3-935144D31425}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>